<commit_message>
Tabela com os dados retirados da uniprot doc.txt
</commit_message>
<xml_diff>
--- a/Resultados/Tabela/info_uniprot.xlsx
+++ b/Resultados/Tabela/info_uniprot.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Varzim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Varzim\Documents\GitHub\Trab_Lab_Algoritmos\Resultados\Tabela\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4650"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="uniprot_d" sheetId="1" r:id="rId1"/>
@@ -2756,8 +2756,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Cor1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3105,3833 +3108,3838 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="44.42578125" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="44.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="86.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1">
+      <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="1" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="1" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="1" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="1" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="1" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="1" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="1" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="1" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="1" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="1" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="1" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="1" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="A85" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="1" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="1" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="1" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="1" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E103" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="A104" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A105" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="A106" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E106" s="1" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="1" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="1" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="A112" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="1" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="1" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E115" s="1" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="1" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="1" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E118" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E119" s="1" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E120" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="A121" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E121" s="1" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="1" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="A124" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="A125" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E125" s="1" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="A126" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="A127" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E127" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="A128" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E128" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E129" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="A130" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E130" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A131" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E131" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="A132" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E132" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E133" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="A134" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D134" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E134" s="1" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E135" s="1" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="A136" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E136" s="1" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="A137" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E137" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="A138" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D138" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E138" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="A139" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E139" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="A140" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="A141" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C141" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D141" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E141" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="A142" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E142" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="A143" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+      <c r="A144" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E144" s="1" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="A145" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E145" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="A146" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E146" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="A147" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E147" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="A148" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E148" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="A149" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E149" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="A150" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E150" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="A151" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E151" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="A152" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C152" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E152" s="1" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="A153" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D153" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="E153" t="s">
+      <c r="E153" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="A154" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C154" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E154" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="A155" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D155" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E155" s="1" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="A156" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D156" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E156" s="1" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+      <c r="A157" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D157" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+      <c r="A158" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E158" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="A159" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D159" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E159" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="A160" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C160" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D160" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E160" s="1" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="A161" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="E161" t="s">
+      <c r="E161" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="A162" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C162" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D162" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E162" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="A163" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C163" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D163" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="E163" t="s">
+      <c r="E163" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="A164" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D164" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E164" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="A165" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="A166" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="A167" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C167" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D167" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="A168" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C168" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D168" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="E168" t="s">
+      <c r="E168" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="A169" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="A170" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C170" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D170" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="A171" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C171" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="D171" t="s">
+      <c r="D171" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="1" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+      <c r="A172" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C172" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D172" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="E172" t="s">
+      <c r="E172" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+      <c r="A173" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C173" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+      <c r="A174" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="E174" t="s">
+      <c r="E174" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="A175" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="1" t="s">
         <v>583</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="E175" t="s">
+      <c r="E175" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="A176" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C176" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E176" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+      <c r="A177" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="1" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+      <c r="A178" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="1" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+      <c r="A179" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C179" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+      <c r="A180" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="1" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+      <c r="A181" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C181" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="1" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="A182" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+      <c r="A183" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+      <c r="A184" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="A185" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+      <c r="A186" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C186" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="E186" t="s">
+      <c r="E186" s="1" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="A187" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="1" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+      <c r="A188" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C188" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="1" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+      <c r="A189" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B189" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C189" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E189" s="1" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="A190" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C190" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="1" t="s">
         <v>633</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="1" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+      <c r="A191" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="E191" t="s">
+      <c r="E191" s="1" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="A192" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C192" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="E192" t="s">
+      <c r="E192" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="A193" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C193" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="E193" t="s">
+      <c r="E193" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="A194" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C194" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="E194" t="s">
+      <c r="E194" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="A195" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D195" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="1" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="A196" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C196" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="A197" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C197" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="E197" t="s">
+      <c r="E197" s="1" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+      <c r="A198" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C198" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E198" s="1" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+      <c r="A199" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C199" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="E199" t="s">
+      <c r="E199" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+      <c r="A200" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C200" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="E200" t="s">
+      <c r="E200" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+      <c r="A201" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B201" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C201" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D201" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="1" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+      <c r="A202" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C202" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+      <c r="A203" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C203" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="1" t="s">
         <v>677</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="1" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+      <c r="A204" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C204" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+      <c r="A205" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C205" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="E205" t="s">
+      <c r="E205" s="1" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+      <c r="A206" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C206" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="E206" t="s">
+      <c r="E206" s="1" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+      <c r="A207" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B207" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C207" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="E207" t="s">
+      <c r="E207" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+      <c r="A208" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="A209" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B209" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C209" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+      <c r="A210" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C210" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="1" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+      <c r="A211" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B211" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C211" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+      <c r="A212" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B212" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C212" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="1" t="s">
         <v>707</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+      <c r="A213" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C213" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D213" s="1" t="s">
         <v>710</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="1" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+      <c r="A214" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C214" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D214" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="1" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+      <c r="A215" s="1" t="s">
         <v>716</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B215" s="1" t="s">
         <v>716</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C215" s="1" t="s">
         <v>717</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D215" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="A216" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B216" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="1" t="s">
         <v>721</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="A217" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C217" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+      <c r="A218" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B218" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C218" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D218" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E218" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+      <c r="A219" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B219" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C219" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D219" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="E219" t="s">
+      <c r="E219" s="1" t="s">
         <v>731</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+      <c r="A220" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B220" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C220" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D220" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="E220" t="s">
+      <c r="E220" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+      <c r="A221" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B221" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C221" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="E221" t="s">
+      <c r="E221" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+      <c r="A222" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B222" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C222" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="D222" t="s">
+      <c r="D222" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+      <c r="A223" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B223" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C223" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D223" t="s">
+      <c r="D223" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="E223" t="s">
+      <c r="E223" s="1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+      <c r="A224" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B224" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C224" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="D224" t="s">
+      <c r="D224" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E224" s="1" t="s">
         <v>747</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+      <c r="A225" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B225" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="C225" t="s">
+      <c r="C225" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="D225" t="s">
+      <c r="D225" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E225" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>